<commit_message>
Update donors_with_dates.xlsx via app on 2025-08-26 11:20:49
</commit_message>
<xml_diff>
--- a/donors_with_dates.xlsx
+++ b/donors_with_dates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16457" windowHeight="6308"/>
+    <workbookView windowWidth="16457" windowHeight="5588"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>Next_Donation_Date</t>
   </si>
   <si>
-    <t>John Doe</t>
+    <t>Mayank Vatsa</t>
   </si>
   <si>
     <t>vatsam82@gmail.com</t>
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55" outlineLevelRow="4" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
Update donors_with_dates.xlsx via app on 2025-08-26 14:48:24
</commit_message>
<xml_diff>
--- a/donors_with_dates.xlsx
+++ b/donors_with_dates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16457" windowHeight="5588"/>
+    <workbookView windowWidth="16457" windowHeight="6308"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>Next_Donation_Date</t>
   </si>
   <si>
-    <t>Mayank Vatsa</t>
+    <t>Rahul</t>
   </si>
   <si>
     <t>vatsam82@gmail.com</t>

</xml_diff>